<commit_message>
creating 6 hour interval rain event dataset.
</commit_message>
<xml_diff>
--- a/data/scratch/armRain_samps.xlsx
+++ b/data/scratch/armRain_samps.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ISU\Project\SoilMove\data\statistics\flume_analysis\data\scratch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ISU\ResearchProject\flume_analysis\data\scratch\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C502CD6-53F0-4C6B-B33C-8A8680EFFD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12108" windowHeight="8928"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="19110" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="armRain_samps" sheetId="1" r:id="rId1"/>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -866,11 +867,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2285"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="A636" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -878,9 +879,10 @@
     <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
wrangling flume and rainfall dataset to see how characterizing runoff and rain changes the results.
</commit_message>
<xml_diff>
--- a/data/scratch/armRain_samps.xlsx
+++ b/data/scratch/armRain_samps.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ISU\Project\SoilMove\data\statistics\flume_analysis\data\scratch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ISU\ResearchProject\flume_analysis\data\scratch\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C502CD6-53F0-4C6B-B33C-8A8680EFFD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12108" windowHeight="8928"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="19110" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="armRain_samps" sheetId="1" r:id="rId1"/>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -866,11 +867,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2285"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="A636" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -878,9 +879,10 @@
     <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>